<commit_message>
Check gl mapping aangepast
</commit_message>
<xml_diff>
--- a/Grootboekschema.xlsx
+++ b/Grootboekschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\HV_PROJECTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB038A-F34F-487D-BC89-FF0DC5D5810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACA6D94-0A1B-4FBB-9754-19901DAF6D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5CC0EE8A-7010-4891-AA6D-14A6785AE550}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5CC0EE8A-7010-4891-AA6D-14A6785AE550}"/>
   </bookViews>
   <sheets>
     <sheet name="Grootboekmapping" sheetId="3" r:id="rId1"/>
@@ -1881,9 +1881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C60EF9-2203-44A3-A11B-517663638815}">
   <dimension ref="A1:L303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J273" sqref="J273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,9 +1966,13 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2" s="5">
+        <f t="shared" ref="K2:K21" si="0">IF(LEN(A2)&lt;5,"0"&amp;A2,A2)</f>
+        <v>80000</v>
+      </c>
       <c r="L2">
         <f>LEN(K2)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2002,9 +2006,13 @@
       <c r="J3">
         <v>2</v>
       </c>
+      <c r="K3" s="5">
+        <f t="shared" si="0"/>
+        <v>80009</v>
+      </c>
       <c r="L3">
-        <f t="shared" ref="L3:L66" si="0">LEN(K3)</f>
-        <v>0</v>
+        <f t="shared" ref="L3:L66" si="1">LEN(K3)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2038,9 +2046,13 @@
       <c r="J4">
         <v>3</v>
       </c>
+      <c r="K4" s="5">
+        <f t="shared" si="0"/>
+        <v>80010</v>
+      </c>
       <c r="L4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2074,9 +2086,13 @@
       <c r="J5">
         <v>4</v>
       </c>
+      <c r="K5" s="5">
+        <f t="shared" si="0"/>
+        <v>80020</v>
+      </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2110,9 +2126,13 @@
       <c r="J6">
         <v>5</v>
       </c>
+      <c r="K6" s="5">
+        <f t="shared" si="0"/>
+        <v>80030</v>
+      </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2146,9 +2166,13 @@
       <c r="J7">
         <v>6</v>
       </c>
+      <c r="K7" s="5">
+        <f t="shared" si="0"/>
+        <v>80040</v>
+      </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2182,9 +2206,13 @@
       <c r="J8">
         <v>7</v>
       </c>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>80500</v>
+      </c>
       <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,9 +2246,13 @@
       <c r="J9">
         <v>8</v>
       </c>
+      <c r="K9" s="5">
+        <f t="shared" si="0"/>
+        <v>89000</v>
+      </c>
       <c r="L9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2254,9 +2286,13 @@
       <c r="J10">
         <v>9</v>
       </c>
+      <c r="K10" s="5">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
       <c r="L10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2290,9 +2326,13 @@
       <c r="J11">
         <v>10</v>
       </c>
+      <c r="K11" s="5">
+        <f t="shared" si="0"/>
+        <v>90020</v>
+      </c>
       <c r="L11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2326,9 +2366,13 @@
       <c r="J12">
         <v>11</v>
       </c>
+      <c r="K12" s="5">
+        <f t="shared" si="0"/>
+        <v>70000</v>
+      </c>
       <c r="L12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2362,9 +2406,13 @@
       <c r="J13">
         <v>12</v>
       </c>
+      <c r="K13" s="5">
+        <f t="shared" si="0"/>
+        <v>70009</v>
+      </c>
       <c r="L13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2398,9 +2446,13 @@
       <c r="J14">
         <v>13</v>
       </c>
+      <c r="K14" s="5">
+        <f t="shared" si="0"/>
+        <v>70010</v>
+      </c>
       <c r="L14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2434,9 +2486,13 @@
       <c r="J15">
         <v>14</v>
       </c>
+      <c r="K15" s="5">
+        <f t="shared" si="0"/>
+        <v>70020</v>
+      </c>
       <c r="L15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2470,9 +2526,13 @@
       <c r="J16">
         <v>15</v>
       </c>
+      <c r="K16" s="5">
+        <f t="shared" si="0"/>
+        <v>70030</v>
+      </c>
       <c r="L16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2506,9 +2566,13 @@
       <c r="J17">
         <v>16</v>
       </c>
+      <c r="K17" s="5">
+        <f t="shared" si="0"/>
+        <v>70040</v>
+      </c>
       <c r="L17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2542,9 +2606,13 @@
       <c r="J18">
         <v>17</v>
       </c>
+      <c r="K18" s="5">
+        <f t="shared" si="0"/>
+        <v>70500</v>
+      </c>
       <c r="L18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2578,9 +2646,13 @@
       <c r="J19">
         <v>18</v>
       </c>
+      <c r="K19" s="5">
+        <f t="shared" si="0"/>
+        <v>79000</v>
+      </c>
       <c r="L19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2614,9 +2686,13 @@
       <c r="J20">
         <v>19</v>
       </c>
+      <c r="K20" s="5">
+        <f t="shared" si="0"/>
+        <v>79010</v>
+      </c>
       <c r="L20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2650,9 +2726,13 @@
       <c r="J21">
         <v>20</v>
       </c>
+      <c r="K21" s="5">
+        <f t="shared" si="0"/>
+        <v>79020</v>
+      </c>
       <c r="L21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2687,11 +2767,11 @@
         <v>21</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" ref="K3:K65" si="1">IF(LEN(A22)&lt;5,"0"&amp;A22,A22)</f>
+        <f t="shared" ref="K22:K65" si="2">IF(LEN(A22)&lt;5,"0"&amp;A22,A22)</f>
         <v>79030</v>
       </c>
       <c r="L22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -2727,11 +2807,11 @@
         <v>22</v>
       </c>
       <c r="K23" s="5">
+        <f t="shared" si="2"/>
+        <v>79100</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="1"/>
-        <v>79100</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2767,11 +2847,11 @@
         <v>23</v>
       </c>
       <c r="K24" s="5">
+        <f t="shared" si="2"/>
+        <v>79110</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="1"/>
-        <v>79110</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2807,11 +2887,11 @@
         <v>24</v>
       </c>
       <c r="K25" s="5">
+        <f t="shared" si="2"/>
+        <v>79120</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="1"/>
-        <v>79120</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2847,11 +2927,11 @@
         <v>25</v>
       </c>
       <c r="K26" s="5">
+        <f t="shared" si="2"/>
+        <v>79130</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="1"/>
-        <v>79130</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2887,11 +2967,11 @@
         <v>26</v>
       </c>
       <c r="K27" s="5">
+        <f t="shared" si="2"/>
+        <v>90010</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="1"/>
-        <v>90010</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2927,11 +3007,11 @@
         <v>27</v>
       </c>
       <c r="K28" s="5">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="1"/>
-        <v>40000</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2967,11 +3047,11 @@
         <v>28</v>
       </c>
       <c r="K29" s="5">
+        <f t="shared" si="2"/>
+        <v>40010</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="1"/>
-        <v>40010</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3007,11 +3087,11 @@
         <v>29</v>
       </c>
       <c r="K30" s="5">
+        <f t="shared" si="2"/>
+        <v>40020</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="1"/>
-        <v>40020</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3047,11 +3127,11 @@
         <v>30</v>
       </c>
       <c r="K31" s="5">
+        <f t="shared" si="2"/>
+        <v>40025</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="1"/>
-        <v>40025</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3087,11 +3167,11 @@
         <v>31</v>
       </c>
       <c r="K32" s="5">
+        <f t="shared" si="2"/>
+        <v>40030</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="1"/>
-        <v>40030</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3127,11 +3207,11 @@
         <v>32</v>
       </c>
       <c r="K33" s="5">
+        <f t="shared" si="2"/>
+        <v>40040</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="1"/>
-        <v>40040</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3167,11 +3247,11 @@
         <v>33</v>
       </c>
       <c r="K34" s="5">
+        <f t="shared" si="2"/>
+        <v>40050</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="1"/>
-        <v>40050</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3207,11 +3287,11 @@
         <v>34</v>
       </c>
       <c r="K35" s="5">
+        <f t="shared" si="2"/>
+        <v>40060</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="1"/>
-        <v>40060</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3247,11 +3327,11 @@
         <v>35</v>
       </c>
       <c r="K36" s="5">
+        <f t="shared" si="2"/>
+        <v>40070</v>
+      </c>
+      <c r="L36">
         <f t="shared" si="1"/>
-        <v>40070</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3287,11 +3367,11 @@
         <v>36</v>
       </c>
       <c r="K37" s="5">
+        <f t="shared" si="2"/>
+        <v>40100</v>
+      </c>
+      <c r="L37">
         <f t="shared" si="1"/>
-        <v>40100</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3327,11 +3407,11 @@
         <v>37</v>
       </c>
       <c r="K38" s="5">
+        <f t="shared" si="2"/>
+        <v>40110</v>
+      </c>
+      <c r="L38">
         <f t="shared" si="1"/>
-        <v>40110</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3367,11 +3447,11 @@
         <v>38</v>
       </c>
       <c r="K39" s="5">
+        <f t="shared" si="2"/>
+        <v>40200</v>
+      </c>
+      <c r="L39">
         <f t="shared" si="1"/>
-        <v>40200</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3407,11 +3487,11 @@
         <v>39</v>
       </c>
       <c r="K40" s="5">
+        <f t="shared" si="2"/>
+        <v>40210</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="1"/>
-        <v>40210</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3447,11 +3527,11 @@
         <v>40</v>
       </c>
       <c r="K41" s="5">
+        <f t="shared" si="2"/>
+        <v>40300</v>
+      </c>
+      <c r="L41">
         <f t="shared" si="1"/>
-        <v>40300</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3487,11 +3567,11 @@
         <v>41</v>
       </c>
       <c r="K42" s="5">
+        <f t="shared" si="2"/>
+        <v>40310</v>
+      </c>
+      <c r="L42">
         <f t="shared" si="1"/>
-        <v>40310</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3527,11 +3607,11 @@
         <v>42</v>
       </c>
       <c r="K43" s="5">
+        <f t="shared" si="2"/>
+        <v>40400</v>
+      </c>
+      <c r="L43">
         <f t="shared" si="1"/>
-        <v>40400</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3567,11 +3647,11 @@
         <v>43</v>
       </c>
       <c r="K44" s="5">
+        <f t="shared" si="2"/>
+        <v>40410</v>
+      </c>
+      <c r="L44">
         <f t="shared" si="1"/>
-        <v>40410</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3607,11 +3687,11 @@
         <v>44</v>
       </c>
       <c r="K45" s="5">
+        <f t="shared" si="2"/>
+        <v>40415</v>
+      </c>
+      <c r="L45">
         <f t="shared" si="1"/>
-        <v>40415</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3647,11 +3727,11 @@
         <v>45</v>
       </c>
       <c r="K46" s="5">
+        <f t="shared" si="2"/>
+        <v>40420</v>
+      </c>
+      <c r="L46">
         <f t="shared" si="1"/>
-        <v>40420</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3687,11 +3767,11 @@
         <v>46</v>
       </c>
       <c r="K47" s="5">
+        <f t="shared" si="2"/>
+        <v>40430</v>
+      </c>
+      <c r="L47">
         <f t="shared" si="1"/>
-        <v>40430</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3727,11 +3807,11 @@
         <v>47</v>
       </c>
       <c r="K48" s="5">
+        <f t="shared" si="2"/>
+        <v>40440</v>
+      </c>
+      <c r="L48">
         <f t="shared" si="1"/>
-        <v>40440</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3767,11 +3847,11 @@
         <v>48</v>
       </c>
       <c r="K49" s="5">
+        <f t="shared" si="2"/>
+        <v>40450</v>
+      </c>
+      <c r="L49">
         <f t="shared" si="1"/>
-        <v>40450</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3807,11 +3887,11 @@
         <v>49</v>
       </c>
       <c r="K50" s="5">
+        <f t="shared" si="2"/>
+        <v>40460</v>
+      </c>
+      <c r="L50">
         <f t="shared" si="1"/>
-        <v>40460</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3847,11 +3927,11 @@
         <v>50</v>
       </c>
       <c r="K51" s="5">
+        <f t="shared" si="2"/>
+        <v>40470</v>
+      </c>
+      <c r="L51">
         <f t="shared" si="1"/>
-        <v>40470</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3887,11 +3967,11 @@
         <v>51</v>
       </c>
       <c r="K52" s="5">
+        <f t="shared" si="2"/>
+        <v>40480</v>
+      </c>
+      <c r="L52">
         <f t="shared" si="1"/>
-        <v>40480</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3927,11 +4007,11 @@
         <v>52</v>
       </c>
       <c r="K53" s="5">
+        <f t="shared" si="2"/>
+        <v>40490</v>
+      </c>
+      <c r="L53">
         <f t="shared" si="1"/>
-        <v>40490</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3967,11 +4047,11 @@
         <v>53</v>
       </c>
       <c r="K54" s="5">
+        <f t="shared" si="2"/>
+        <v>40495</v>
+      </c>
+      <c r="L54">
         <f t="shared" si="1"/>
-        <v>40495</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4007,11 +4087,11 @@
         <v>54</v>
       </c>
       <c r="K55" s="5">
+        <f t="shared" si="2"/>
+        <v>41000</v>
+      </c>
+      <c r="L55">
         <f t="shared" si="1"/>
-        <v>41000</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4047,11 +4127,11 @@
         <v>55</v>
       </c>
       <c r="K56" s="5">
+        <f t="shared" si="2"/>
+        <v>41005</v>
+      </c>
+      <c r="L56">
         <f t="shared" si="1"/>
-        <v>41005</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4087,11 +4167,11 @@
         <v>56</v>
       </c>
       <c r="K57" s="5">
+        <f t="shared" si="2"/>
+        <v>41010</v>
+      </c>
+      <c r="L57">
         <f t="shared" si="1"/>
-        <v>41010</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4127,11 +4207,11 @@
         <v>57</v>
       </c>
       <c r="K58" s="5">
+        <f t="shared" si="2"/>
+        <v>41020</v>
+      </c>
+      <c r="L58">
         <f t="shared" si="1"/>
-        <v>41020</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4167,11 +4247,11 @@
         <v>58</v>
       </c>
       <c r="K59" s="5">
+        <f t="shared" si="2"/>
+        <v>41030</v>
+      </c>
+      <c r="L59">
         <f t="shared" si="1"/>
-        <v>41030</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4207,11 +4287,11 @@
         <v>59</v>
       </c>
       <c r="K60" s="5">
+        <f t="shared" si="2"/>
+        <v>41040</v>
+      </c>
+      <c r="L60">
         <f t="shared" si="1"/>
-        <v>41040</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4247,11 +4327,11 @@
         <v>60</v>
       </c>
       <c r="K61" s="5">
+        <f t="shared" si="2"/>
+        <v>41050</v>
+      </c>
+      <c r="L61">
         <f t="shared" si="1"/>
-        <v>41050</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4287,11 +4367,11 @@
         <v>61</v>
       </c>
       <c r="K62" s="5">
+        <f t="shared" si="2"/>
+        <v>42000</v>
+      </c>
+      <c r="L62">
         <f t="shared" si="1"/>
-        <v>42000</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4327,11 +4407,11 @@
         <v>62</v>
       </c>
       <c r="K63" s="5">
+        <f t="shared" si="2"/>
+        <v>42010</v>
+      </c>
+      <c r="L63">
         <f t="shared" si="1"/>
-        <v>42010</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4367,11 +4447,11 @@
         <v>63</v>
       </c>
       <c r="K64" s="5">
+        <f t="shared" si="2"/>
+        <v>42020</v>
+      </c>
+      <c r="L64">
         <f t="shared" si="1"/>
-        <v>42020</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4407,11 +4487,11 @@
         <v>64</v>
       </c>
       <c r="K65" s="5">
+        <f t="shared" si="2"/>
+        <v>42030</v>
+      </c>
+      <c r="L65">
         <f t="shared" si="1"/>
-        <v>42030</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -4447,11 +4527,11 @@
         <v>65</v>
       </c>
       <c r="K66" s="5">
-        <f t="shared" ref="K66:K129" si="2">IF(LEN(A66)&lt;5,"0"&amp;A66,A66)</f>
+        <f t="shared" ref="K66:K129" si="3">IF(LEN(A66)&lt;5,"0"&amp;A66,A66)</f>
         <v>42040</v>
       </c>
       <c r="L66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -4487,11 +4567,11 @@
         <v>66</v>
       </c>
       <c r="K67" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42050</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L130" si="3">LEN(K67)</f>
+        <f t="shared" ref="L67:L130" si="4">LEN(K67)</f>
         <v>5</v>
       </c>
     </row>
@@ -4527,11 +4607,11 @@
         <v>67</v>
       </c>
       <c r="K68" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42060</v>
       </c>
       <c r="L68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4567,11 +4647,11 @@
         <v>68</v>
       </c>
       <c r="K69" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42070</v>
       </c>
       <c r="L69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4607,11 +4687,11 @@
         <v>69</v>
       </c>
       <c r="K70" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42090</v>
       </c>
       <c r="L70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4647,11 +4727,11 @@
         <v>70</v>
       </c>
       <c r="K71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42095</v>
       </c>
       <c r="L71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4687,11 +4767,11 @@
         <v>71</v>
       </c>
       <c r="K72" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42500</v>
       </c>
       <c r="L72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4727,11 +4807,11 @@
         <v>72</v>
       </c>
       <c r="K73" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42510</v>
       </c>
       <c r="L73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4767,11 +4847,11 @@
         <v>73</v>
       </c>
       <c r="K74" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42520</v>
       </c>
       <c r="L74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4807,11 +4887,11 @@
         <v>74</v>
       </c>
       <c r="K75" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42530</v>
       </c>
       <c r="L75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4847,11 +4927,11 @@
         <v>75</v>
       </c>
       <c r="K76" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42540</v>
       </c>
       <c r="L76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4887,11 +4967,11 @@
         <v>76</v>
       </c>
       <c r="K77" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42550</v>
       </c>
       <c r="L77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4927,11 +5007,11 @@
         <v>77</v>
       </c>
       <c r="K78" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42560</v>
       </c>
       <c r="L78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -4967,11 +5047,11 @@
         <v>78</v>
       </c>
       <c r="K79" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42590</v>
       </c>
       <c r="L79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5007,11 +5087,11 @@
         <v>79</v>
       </c>
       <c r="K80" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42595</v>
       </c>
       <c r="L80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5047,11 +5127,11 @@
         <v>80</v>
       </c>
       <c r="K81" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43000</v>
       </c>
       <c r="L81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5087,11 +5167,11 @@
         <v>81</v>
       </c>
       <c r="K82" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43010</v>
       </c>
       <c r="L82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5127,11 +5207,11 @@
         <v>82</v>
       </c>
       <c r="K83" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43020</v>
       </c>
       <c r="L83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5167,11 +5247,11 @@
         <v>83</v>
       </c>
       <c r="K84" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43030</v>
       </c>
       <c r="L84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5207,11 +5287,11 @@
         <v>84</v>
       </c>
       <c r="K85" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43040</v>
       </c>
       <c r="L85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5247,11 +5327,11 @@
         <v>85</v>
       </c>
       <c r="K86" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43050</v>
       </c>
       <c r="L86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5287,11 +5367,11 @@
         <v>86</v>
       </c>
       <c r="K87" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43060</v>
       </c>
       <c r="L87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5327,11 +5407,11 @@
         <v>87</v>
       </c>
       <c r="K88" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43090</v>
       </c>
       <c r="L88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5367,11 +5447,11 @@
         <v>88</v>
       </c>
       <c r="K89" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43095</v>
       </c>
       <c r="L89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5407,11 +5487,11 @@
         <v>89</v>
       </c>
       <c r="K90" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44000</v>
       </c>
       <c r="L90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5447,11 +5527,11 @@
         <v>90</v>
       </c>
       <c r="K91" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44010</v>
       </c>
       <c r="L91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5487,11 +5567,11 @@
         <v>91</v>
       </c>
       <c r="K92" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44020</v>
       </c>
       <c r="L92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5527,11 +5607,11 @@
         <v>92</v>
       </c>
       <c r="K93" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44030</v>
       </c>
       <c r="L93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5567,11 +5647,11 @@
         <v>93</v>
       </c>
       <c r="K94" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44040</v>
       </c>
       <c r="L94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5607,11 +5687,11 @@
         <v>94</v>
       </c>
       <c r="K95" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44050</v>
       </c>
       <c r="L95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5647,11 +5727,11 @@
         <v>95</v>
       </c>
       <c r="K96" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44060</v>
       </c>
       <c r="L96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5687,11 +5767,11 @@
         <v>96</v>
       </c>
       <c r="K97" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44080</v>
       </c>
       <c r="L97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5727,11 +5807,11 @@
         <v>97</v>
       </c>
       <c r="K98" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44090</v>
       </c>
       <c r="L98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5767,11 +5847,11 @@
         <v>98</v>
       </c>
       <c r="K99" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44095</v>
       </c>
       <c r="L99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5807,11 +5887,11 @@
         <v>99</v>
       </c>
       <c r="K100" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45200</v>
       </c>
       <c r="L100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5847,11 +5927,11 @@
         <v>100</v>
       </c>
       <c r="K101" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45210</v>
       </c>
       <c r="L101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5887,11 +5967,11 @@
         <v>101</v>
       </c>
       <c r="K102" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46000</v>
       </c>
       <c r="L102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5927,11 +6007,11 @@
         <v>102</v>
       </c>
       <c r="K103" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46010</v>
       </c>
       <c r="L103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -5967,11 +6047,11 @@
         <v>103</v>
       </c>
       <c r="K104" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46020</v>
       </c>
       <c r="L104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6007,11 +6087,11 @@
         <v>104</v>
       </c>
       <c r="K105" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46090</v>
       </c>
       <c r="L105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6047,11 +6127,11 @@
         <v>105</v>
       </c>
       <c r="K106" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46095</v>
       </c>
       <c r="L106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6087,11 +6167,11 @@
         <v>106</v>
       </c>
       <c r="K107" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49000</v>
       </c>
       <c r="L107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6127,11 +6207,11 @@
         <v>107</v>
       </c>
       <c r="K108" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49010</v>
       </c>
       <c r="L108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6167,11 +6247,11 @@
         <v>108</v>
       </c>
       <c r="K109" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49020</v>
       </c>
       <c r="L109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6207,11 +6287,11 @@
         <v>109</v>
       </c>
       <c r="K110" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49030</v>
       </c>
       <c r="L110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6247,11 +6327,11 @@
         <v>110</v>
       </c>
       <c r="K111" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49090</v>
       </c>
       <c r="L111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6287,11 +6367,11 @@
         <v>111</v>
       </c>
       <c r="K112" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49095</v>
       </c>
       <c r="L112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6327,11 +6407,11 @@
         <v>112</v>
       </c>
       <c r="K113" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45040</v>
       </c>
       <c r="L113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6367,11 +6447,11 @@
         <v>113</v>
       </c>
       <c r="K114" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45000</v>
       </c>
       <c r="L114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6407,11 +6487,11 @@
         <v>114</v>
       </c>
       <c r="K115" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45010</v>
       </c>
       <c r="L115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6447,11 +6527,11 @@
         <v>115</v>
       </c>
       <c r="K116" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45100</v>
       </c>
       <c r="L116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6487,11 +6567,11 @@
         <v>116</v>
       </c>
       <c r="K117" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45110</v>
       </c>
       <c r="L117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6527,11 +6607,11 @@
         <v>117</v>
       </c>
       <c r="K118" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45120</v>
       </c>
       <c r="L118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6567,11 +6647,11 @@
         <v>118</v>
       </c>
       <c r="K119" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45130</v>
       </c>
       <c r="L119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6607,11 +6687,11 @@
         <v>119</v>
       </c>
       <c r="K120" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47000</v>
       </c>
       <c r="L120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6647,11 +6727,11 @@
         <v>120</v>
       </c>
       <c r="K121" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47010</v>
       </c>
       <c r="L121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6687,11 +6767,11 @@
         <v>121</v>
       </c>
       <c r="K122" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47020</v>
       </c>
       <c r="L122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6727,11 +6807,11 @@
         <v>122</v>
       </c>
       <c r="K123" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47030</v>
       </c>
       <c r="L123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6767,11 +6847,11 @@
         <v>123</v>
       </c>
       <c r="K124" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47040</v>
       </c>
       <c r="L124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6807,11 +6887,11 @@
         <v>124</v>
       </c>
       <c r="K125" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47050</v>
       </c>
       <c r="L125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6847,11 +6927,11 @@
         <v>125</v>
       </c>
       <c r="K126" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47060</v>
       </c>
       <c r="L126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6887,11 +6967,11 @@
         <v>126</v>
       </c>
       <c r="K127" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47090</v>
       </c>
       <c r="L127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6927,11 +7007,11 @@
         <v>127</v>
       </c>
       <c r="K128" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47095</v>
       </c>
       <c r="L128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -6967,11 +7047,11 @@
         <v>128</v>
       </c>
       <c r="K129" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47100</v>
       </c>
       <c r="L129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -7007,11 +7087,11 @@
         <v>129</v>
       </c>
       <c r="K130" s="5">
-        <f t="shared" ref="K130:K133" si="4">IF(LEN(A130)&lt;5,"0"&amp;A130,A130)</f>
+        <f t="shared" ref="K130:K133" si="5">IF(LEN(A130)&lt;5,"0"&amp;A130,A130)</f>
         <v>47110</v>
       </c>
       <c r="L130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -7047,11 +7127,11 @@
         <v>130</v>
       </c>
       <c r="K131" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47120</v>
       </c>
       <c r="L131">
-        <f t="shared" ref="L131:L194" si="5">LEN(K131)</f>
+        <f t="shared" ref="L131:L194" si="6">LEN(K131)</f>
         <v>5</v>
       </c>
     </row>
@@ -7087,11 +7167,11 @@
         <v>131</v>
       </c>
       <c r="K132" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47130</v>
       </c>
       <c r="L132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -7127,11 +7207,11 @@
         <v>132</v>
       </c>
       <c r="K133" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47140</v>
       </c>
       <c r="L133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -7171,7 +7251,7 @@
         <v>47150</v>
       </c>
       <c r="L134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -7207,11 +7287,11 @@
         <v>134</v>
       </c>
       <c r="K135" s="5">
-        <f t="shared" ref="K135:K198" si="6">IF(LEN(A135)&lt;5,"0"&amp;A135,A135)</f>
+        <f t="shared" ref="K135:K198" si="7">IF(LEN(A135)&lt;5,"0"&amp;A135,A135)</f>
         <v>47195</v>
       </c>
       <c r="L135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -7247,11 +7327,11 @@
         <v>135</v>
       </c>
       <c r="K136" s="5">
+        <f t="shared" si="7"/>
+        <v>49920</v>
+      </c>
+      <c r="L136">
         <f t="shared" si="6"/>
-        <v>49920</v>
-      </c>
-      <c r="L136">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7287,11 +7367,11 @@
         <v>136</v>
       </c>
       <c r="K137" s="5">
+        <f t="shared" si="7"/>
+        <v>49930</v>
+      </c>
+      <c r="L137">
         <f t="shared" si="6"/>
-        <v>49930</v>
-      </c>
-      <c r="L137">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7327,11 +7407,11 @@
         <v>137</v>
       </c>
       <c r="K138" s="5">
+        <f t="shared" si="7"/>
+        <v>49940</v>
+      </c>
+      <c r="L138">
         <f t="shared" si="6"/>
-        <v>49940</v>
-      </c>
-      <c r="L138">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7367,11 +7447,11 @@
         <v>138</v>
       </c>
       <c r="K139" s="5">
+        <f t="shared" si="7"/>
+        <v>49950</v>
+      </c>
+      <c r="L139">
         <f t="shared" si="6"/>
-        <v>49950</v>
-      </c>
-      <c r="L139">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7407,11 +7487,11 @@
         <v>139</v>
       </c>
       <c r="K140" s="5">
+        <f t="shared" si="7"/>
+        <v>49990</v>
+      </c>
+      <c r="L140">
         <f t="shared" si="6"/>
-        <v>49990</v>
-      </c>
-      <c r="L140">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7447,11 +7527,11 @@
         <v>140</v>
       </c>
       <c r="K141" s="5">
+        <f t="shared" si="7"/>
+        <v>49995</v>
+      </c>
+      <c r="L141">
         <f t="shared" si="6"/>
-        <v>49995</v>
-      </c>
-      <c r="L141">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7487,11 +7567,11 @@
         <v>141</v>
       </c>
       <c r="K142" s="5">
+        <f t="shared" si="7"/>
+        <v>48000</v>
+      </c>
+      <c r="L142">
         <f t="shared" si="6"/>
-        <v>48000</v>
-      </c>
-      <c r="L142">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7527,11 +7607,11 @@
         <v>142</v>
       </c>
       <c r="K143" s="5">
+        <f t="shared" si="7"/>
+        <v>48010</v>
+      </c>
+      <c r="L143">
         <f t="shared" si="6"/>
-        <v>48010</v>
-      </c>
-      <c r="L143">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7567,11 +7647,11 @@
         <v>143</v>
       </c>
       <c r="K144" s="5">
+        <f t="shared" si="7"/>
+        <v>48020</v>
+      </c>
+      <c r="L144">
         <f t="shared" si="6"/>
-        <v>48020</v>
-      </c>
-      <c r="L144">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7607,11 +7687,11 @@
         <v>144</v>
       </c>
       <c r="K145" s="5">
+        <f t="shared" si="7"/>
+        <v>48030</v>
+      </c>
+      <c r="L145">
         <f t="shared" si="6"/>
-        <v>48030</v>
-      </c>
-      <c r="L145">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7647,11 +7727,11 @@
         <v>145</v>
       </c>
       <c r="K146" s="5">
+        <f t="shared" si="7"/>
+        <v>48040</v>
+      </c>
+      <c r="L146">
         <f t="shared" si="6"/>
-        <v>48040</v>
-      </c>
-      <c r="L146">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7687,11 +7767,11 @@
         <v>146</v>
       </c>
       <c r="K147" s="5">
+        <f t="shared" si="7"/>
+        <v>48090</v>
+      </c>
+      <c r="L147">
         <f t="shared" si="6"/>
-        <v>48090</v>
-      </c>
-      <c r="L147">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7727,11 +7807,11 @@
         <v>147</v>
       </c>
       <c r="K148" s="5">
+        <f t="shared" si="7"/>
+        <v>49900</v>
+      </c>
+      <c r="L148">
         <f t="shared" si="6"/>
-        <v>49900</v>
-      </c>
-      <c r="L148">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7767,11 +7847,11 @@
         <v>148</v>
       </c>
       <c r="K149" s="5">
+        <f t="shared" si="7"/>
+        <v>49910</v>
+      </c>
+      <c r="L149">
         <f t="shared" si="6"/>
-        <v>49910</v>
-      </c>
-      <c r="L149">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7807,11 +7887,11 @@
         <v>149</v>
       </c>
       <c r="K150" s="5">
+        <f t="shared" si="7"/>
+        <v>45050</v>
+      </c>
+      <c r="L150">
         <f t="shared" si="6"/>
-        <v>45050</v>
-      </c>
-      <c r="L150">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7847,11 +7927,11 @@
         <v>150</v>
       </c>
       <c r="K151" s="5">
+        <f t="shared" si="7"/>
+        <v>60000</v>
+      </c>
+      <c r="L151">
         <f t="shared" si="6"/>
-        <v>60000</v>
-      </c>
-      <c r="L151">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7887,11 +7967,11 @@
         <v>151</v>
       </c>
       <c r="K152" s="5">
+        <f t="shared" si="7"/>
+        <v>60020</v>
+      </c>
+      <c r="L152">
         <f t="shared" si="6"/>
-        <v>60020</v>
-      </c>
-      <c r="L152">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7927,11 +8007,11 @@
         <v>152</v>
       </c>
       <c r="K153" s="5">
+        <f t="shared" si="7"/>
+        <v>60030</v>
+      </c>
+      <c r="L153">
         <f t="shared" si="6"/>
-        <v>60030</v>
-      </c>
-      <c r="L153">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -7967,11 +8047,11 @@
         <v>153</v>
       </c>
       <c r="K154" s="5">
+        <f t="shared" si="7"/>
+        <v>60040</v>
+      </c>
+      <c r="L154">
         <f t="shared" si="6"/>
-        <v>60040</v>
-      </c>
-      <c r="L154">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8007,11 +8087,11 @@
         <v>154</v>
       </c>
       <c r="K155" s="5">
+        <f t="shared" si="7"/>
+        <v>60050</v>
+      </c>
+      <c r="L155">
         <f t="shared" si="6"/>
-        <v>60050</v>
-      </c>
-      <c r="L155">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8047,11 +8127,11 @@
         <v>155</v>
       </c>
       <c r="K156" s="5">
+        <f t="shared" si="7"/>
+        <v>60090</v>
+      </c>
+      <c r="L156">
         <f t="shared" si="6"/>
-        <v>60090</v>
-      </c>
-      <c r="L156">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8087,11 +8167,11 @@
         <v>156</v>
       </c>
       <c r="K157" s="5">
+        <f t="shared" si="7"/>
+        <v>61000</v>
+      </c>
+      <c r="L157">
         <f t="shared" si="6"/>
-        <v>61000</v>
-      </c>
-      <c r="L157">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8127,11 +8207,11 @@
         <v>157</v>
       </c>
       <c r="K158" s="5">
+        <f t="shared" si="7"/>
+        <v>61010</v>
+      </c>
+      <c r="L158">
         <f t="shared" si="6"/>
-        <v>61010</v>
-      </c>
-      <c r="L158">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8167,11 +8247,11 @@
         <v>158</v>
       </c>
       <c r="K159" s="5">
+        <f t="shared" si="7"/>
+        <v>91000</v>
+      </c>
+      <c r="L159">
         <f t="shared" si="6"/>
-        <v>91000</v>
-      </c>
-      <c r="L159">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8207,11 +8287,11 @@
         <v>159</v>
       </c>
       <c r="K160" s="5">
+        <f t="shared" si="7"/>
+        <v>62000</v>
+      </c>
+      <c r="L160">
         <f t="shared" si="6"/>
-        <v>62000</v>
-      </c>
-      <c r="L160">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8247,11 +8327,11 @@
         <v>160</v>
       </c>
       <c r="K161" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>01000</v>
+      </c>
+      <c r="L161">
         <f t="shared" si="6"/>
-        <v>01000</v>
-      </c>
-      <c r="L161">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8287,11 +8367,11 @@
         <v>161</v>
       </c>
       <c r="K162" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>01010</v>
+      </c>
+      <c r="L162">
         <f t="shared" si="6"/>
-        <v>01010</v>
-      </c>
-      <c r="L162">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8327,11 +8407,11 @@
         <v>162</v>
       </c>
       <c r="K163" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>01500</v>
+      </c>
+      <c r="L163">
         <f t="shared" si="6"/>
-        <v>01500</v>
-      </c>
-      <c r="L163">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8367,11 +8447,11 @@
         <v>163</v>
       </c>
       <c r="K164" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>01510</v>
+      </c>
+      <c r="L164">
         <f t="shared" si="6"/>
-        <v>01510</v>
-      </c>
-      <c r="L164">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8407,11 +8487,11 @@
         <v>164</v>
       </c>
       <c r="K165" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02000</v>
+      </c>
+      <c r="L165">
         <f t="shared" si="6"/>
-        <v>02000</v>
-      </c>
-      <c r="L165">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8447,11 +8527,11 @@
         <v>165</v>
       </c>
       <c r="K166" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02010</v>
+      </c>
+      <c r="L166">
         <f t="shared" si="6"/>
-        <v>02010</v>
-      </c>
-      <c r="L166">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8487,11 +8567,11 @@
         <v>166</v>
       </c>
       <c r="K167" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02300</v>
+      </c>
+      <c r="L167">
         <f t="shared" si="6"/>
-        <v>02300</v>
-      </c>
-      <c r="L167">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8527,11 +8607,11 @@
         <v>167</v>
       </c>
       <c r="K168" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02310</v>
+      </c>
+      <c r="L168">
         <f t="shared" si="6"/>
-        <v>02310</v>
-      </c>
-      <c r="L168">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8567,11 +8647,11 @@
         <v>168</v>
       </c>
       <c r="K169" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02100</v>
+      </c>
+      <c r="L169">
         <f t="shared" si="6"/>
-        <v>02100</v>
-      </c>
-      <c r="L169">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8607,11 +8687,11 @@
         <v>169</v>
       </c>
       <c r="K170" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02110</v>
+      </c>
+      <c r="L170">
         <f t="shared" si="6"/>
-        <v>02110</v>
-      </c>
-      <c r="L170">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8647,11 +8727,11 @@
         <v>170</v>
       </c>
       <c r="K171" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02200</v>
+      </c>
+      <c r="L171">
         <f t="shared" si="6"/>
-        <v>02200</v>
-      </c>
-      <c r="L171">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8687,11 +8767,11 @@
         <v>171</v>
       </c>
       <c r="K172" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>02210</v>
+      </c>
+      <c r="L172">
         <f t="shared" si="6"/>
-        <v>02210</v>
-      </c>
-      <c r="L172">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8727,11 +8807,11 @@
         <v>172</v>
       </c>
       <c r="K173" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06010</v>
+      </c>
+      <c r="L173">
         <f t="shared" si="6"/>
-        <v>06010</v>
-      </c>
-      <c r="L173">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8767,11 +8847,11 @@
         <v>173</v>
       </c>
       <c r="K174" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06011</v>
+      </c>
+      <c r="L174">
         <f t="shared" si="6"/>
-        <v>06011</v>
-      </c>
-      <c r="L174">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8807,11 +8887,11 @@
         <v>174</v>
       </c>
       <c r="K175" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06012</v>
+      </c>
+      <c r="L175">
         <f t="shared" si="6"/>
-        <v>06012</v>
-      </c>
-      <c r="L175">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8847,11 +8927,11 @@
         <v>175</v>
       </c>
       <c r="K176" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06013</v>
+      </c>
+      <c r="L176">
         <f t="shared" si="6"/>
-        <v>06013</v>
-      </c>
-      <c r="L176">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8887,11 +8967,11 @@
         <v>176</v>
       </c>
       <c r="K177" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06014</v>
+      </c>
+      <c r="L177">
         <f t="shared" si="6"/>
-        <v>06014</v>
-      </c>
-      <c r="L177">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8927,11 +9007,11 @@
         <v>177</v>
       </c>
       <c r="K178" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06017</v>
+      </c>
+      <c r="L178">
         <f t="shared" si="6"/>
-        <v>06017</v>
-      </c>
-      <c r="L178">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -8967,11 +9047,11 @@
         <v>178</v>
       </c>
       <c r="K179" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>06018</v>
+      </c>
+      <c r="L179">
         <f t="shared" si="6"/>
-        <v>06018</v>
-      </c>
-      <c r="L179">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9007,11 +9087,11 @@
         <v>179</v>
       </c>
       <c r="K180" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03400</v>
+      </c>
+      <c r="L180">
         <f t="shared" si="6"/>
-        <v>03400</v>
-      </c>
-      <c r="L180">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9047,11 +9127,11 @@
         <v>180</v>
       </c>
       <c r="K181" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03401</v>
+      </c>
+      <c r="L181">
         <f t="shared" si="6"/>
-        <v>03401</v>
-      </c>
-      <c r="L181">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9087,11 +9167,11 @@
         <v>181</v>
       </c>
       <c r="K182" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03402</v>
+      </c>
+      <c r="L182">
         <f t="shared" si="6"/>
-        <v>03402</v>
-      </c>
-      <c r="L182">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9127,11 +9207,11 @@
         <v>182</v>
       </c>
       <c r="K183" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03403</v>
+      </c>
+      <c r="L183">
         <f t="shared" si="6"/>
-        <v>03403</v>
-      </c>
-      <c r="L183">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9167,11 +9247,11 @@
         <v>183</v>
       </c>
       <c r="K184" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03411</v>
+      </c>
+      <c r="L184">
         <f t="shared" si="6"/>
-        <v>03411</v>
-      </c>
-      <c r="L184">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9207,11 +9287,11 @@
         <v>184</v>
       </c>
       <c r="K185" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03413</v>
+      </c>
+      <c r="L185">
         <f t="shared" si="6"/>
-        <v>03413</v>
-      </c>
-      <c r="L185">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9247,11 +9327,11 @@
         <v>185</v>
       </c>
       <c r="K186" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03414</v>
+      </c>
+      <c r="L186">
         <f t="shared" si="6"/>
-        <v>03414</v>
-      </c>
-      <c r="L186">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9287,11 +9367,11 @@
         <v>186</v>
       </c>
       <c r="K187" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03416</v>
+      </c>
+      <c r="L187">
         <f t="shared" si="6"/>
-        <v>03416</v>
-      </c>
-      <c r="L187">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9327,11 +9407,11 @@
         <v>187</v>
       </c>
       <c r="K188" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03417</v>
+      </c>
+      <c r="L188">
         <f t="shared" si="6"/>
-        <v>03417</v>
-      </c>
-      <c r="L188">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9367,11 +9447,11 @@
         <v>188</v>
       </c>
       <c r="K189" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03418</v>
+      </c>
+      <c r="L189">
         <f t="shared" si="6"/>
-        <v>03418</v>
-      </c>
-      <c r="L189">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9407,11 +9487,11 @@
         <v>189</v>
       </c>
       <c r="K190" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03419</v>
+      </c>
+      <c r="L190">
         <f t="shared" si="6"/>
-        <v>03419</v>
-      </c>
-      <c r="L190">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9447,11 +9527,11 @@
         <v>190</v>
       </c>
       <c r="K191" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03420</v>
+      </c>
+      <c r="L191">
         <f t="shared" si="6"/>
-        <v>03420</v>
-      </c>
-      <c r="L191">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9487,11 +9567,11 @@
         <v>191</v>
       </c>
       <c r="K192" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03500</v>
+      </c>
+      <c r="L192">
         <f t="shared" si="6"/>
-        <v>03500</v>
-      </c>
-      <c r="L192">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9527,11 +9607,11 @@
         <v>192</v>
       </c>
       <c r="K193" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03501</v>
+      </c>
+      <c r="L193">
         <f t="shared" si="6"/>
-        <v>03501</v>
-      </c>
-      <c r="L193">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9567,11 +9647,11 @@
         <v>193</v>
       </c>
       <c r="K194" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>03507</v>
+      </c>
+      <c r="L194">
         <f t="shared" si="6"/>
-        <v>03507</v>
-      </c>
-      <c r="L194">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -9607,11 +9687,11 @@
         <v>194</v>
       </c>
       <c r="K195" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03510</v>
       </c>
       <c r="L195">
-        <f t="shared" ref="L195:L258" si="7">LEN(K195)</f>
+        <f t="shared" ref="L195:L258" si="8">LEN(K195)</f>
         <v>5</v>
       </c>
     </row>
@@ -9647,11 +9727,11 @@
         <v>195</v>
       </c>
       <c r="K196" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11000</v>
       </c>
       <c r="L196">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -9687,11 +9767,11 @@
         <v>196</v>
       </c>
       <c r="K197" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11010</v>
       </c>
       <c r="L197">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -9727,11 +9807,11 @@
         <v>197</v>
       </c>
       <c r="K198" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11020</v>
       </c>
       <c r="L198">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -9767,11 +9847,11 @@
         <v>198</v>
       </c>
       <c r="K199" s="5">
-        <f t="shared" ref="K199:K262" si="8">IF(LEN(A199)&lt;5,"0"&amp;A199,A199)</f>
+        <f t="shared" ref="K199:K262" si="9">IF(LEN(A199)&lt;5,"0"&amp;A199,A199)</f>
         <v>11030</v>
       </c>
       <c r="L199">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -9807,11 +9887,11 @@
         <v>199</v>
       </c>
       <c r="K200" s="5">
+        <f t="shared" si="9"/>
+        <v>11040</v>
+      </c>
+      <c r="L200">
         <f t="shared" si="8"/>
-        <v>11040</v>
-      </c>
-      <c r="L200">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -9847,11 +9927,11 @@
         <v>200</v>
       </c>
       <c r="K201" s="5">
+        <f t="shared" si="9"/>
+        <v>11050</v>
+      </c>
+      <c r="L201">
         <f t="shared" si="8"/>
-        <v>11050</v>
-      </c>
-      <c r="L201">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -9887,11 +9967,11 @@
         <v>201</v>
       </c>
       <c r="K202" s="5">
+        <f t="shared" si="9"/>
+        <v>11099</v>
+      </c>
+      <c r="L202">
         <f t="shared" si="8"/>
-        <v>11099</v>
-      </c>
-      <c r="L202">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -9927,11 +10007,11 @@
         <v>202</v>
       </c>
       <c r="K203" s="5">
+        <f t="shared" si="9"/>
+        <v>11100</v>
+      </c>
+      <c r="L203">
         <f t="shared" si="8"/>
-        <v>11100</v>
-      </c>
-      <c r="L203">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -9967,11 +10047,11 @@
         <v>203</v>
       </c>
       <c r="K204" s="5">
+        <f t="shared" si="9"/>
+        <v>11200</v>
+      </c>
+      <c r="L204">
         <f t="shared" si="8"/>
-        <v>11200</v>
-      </c>
-      <c r="L204">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10007,11 +10087,11 @@
         <v>204</v>
       </c>
       <c r="K205" s="5">
+        <f t="shared" si="9"/>
+        <v>15000</v>
+      </c>
+      <c r="L205">
         <f t="shared" si="8"/>
-        <v>15000</v>
-      </c>
-      <c r="L205">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10047,11 +10127,11 @@
         <v>205</v>
       </c>
       <c r="K206" s="5">
+        <f t="shared" si="9"/>
+        <v>15010</v>
+      </c>
+      <c r="L206">
         <f t="shared" si="8"/>
-        <v>15010</v>
-      </c>
-      <c r="L206">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10087,11 +10167,11 @@
         <v>206</v>
       </c>
       <c r="K207" s="5">
+        <f t="shared" si="9"/>
+        <v>15015</v>
+      </c>
+      <c r="L207">
         <f t="shared" si="8"/>
-        <v>15015</v>
-      </c>
-      <c r="L207">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10127,11 +10207,11 @@
         <v>207</v>
       </c>
       <c r="K208" s="5">
+        <f t="shared" si="9"/>
+        <v>15020</v>
+      </c>
+      <c r="L208">
         <f t="shared" si="8"/>
-        <v>15020</v>
-      </c>
-      <c r="L208">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10167,11 +10247,11 @@
         <v>208</v>
       </c>
       <c r="K209" s="5">
+        <f t="shared" si="9"/>
+        <v>15030</v>
+      </c>
+      <c r="L209">
         <f t="shared" si="8"/>
-        <v>15030</v>
-      </c>
-      <c r="L209">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10207,11 +10287,11 @@
         <v>209</v>
       </c>
       <c r="K210" s="5">
+        <f t="shared" si="9"/>
+        <v>15040</v>
+      </c>
+      <c r="L210">
         <f t="shared" si="8"/>
-        <v>15040</v>
-      </c>
-      <c r="L210">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10247,11 +10327,11 @@
         <v>210</v>
       </c>
       <c r="K211" s="5">
+        <f t="shared" si="9"/>
+        <v>15050</v>
+      </c>
+      <c r="L211">
         <f t="shared" si="8"/>
-        <v>15050</v>
-      </c>
-      <c r="L211">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10287,11 +10367,11 @@
         <v>211</v>
       </c>
       <c r="K212" s="5">
+        <f t="shared" si="9"/>
+        <v>15055</v>
+      </c>
+      <c r="L212">
         <f t="shared" si="8"/>
-        <v>15055</v>
-      </c>
-      <c r="L212">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10327,11 +10407,11 @@
         <v>212</v>
       </c>
       <c r="K213" s="5">
+        <f t="shared" si="9"/>
+        <v>15060</v>
+      </c>
+      <c r="L213">
         <f t="shared" si="8"/>
-        <v>15060</v>
-      </c>
-      <c r="L213">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10367,11 +10447,11 @@
         <v>213</v>
       </c>
       <c r="K214" s="5">
+        <f t="shared" si="9"/>
+        <v>15070</v>
+      </c>
+      <c r="L214">
         <f t="shared" si="8"/>
-        <v>15070</v>
-      </c>
-      <c r="L214">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10407,11 +10487,11 @@
         <v>214</v>
       </c>
       <c r="K215" s="5">
+        <f t="shared" si="9"/>
+        <v>16100</v>
+      </c>
+      <c r="L215">
         <f t="shared" si="8"/>
-        <v>16100</v>
-      </c>
-      <c r="L215">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10447,11 +10527,11 @@
         <v>215</v>
       </c>
       <c r="K216" s="5">
+        <f t="shared" si="9"/>
+        <v>16110</v>
+      </c>
+      <c r="L216">
         <f t="shared" si="8"/>
-        <v>16110</v>
-      </c>
-      <c r="L216">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10487,11 +10567,11 @@
         <v>216</v>
       </c>
       <c r="K217" s="5">
+        <f t="shared" si="9"/>
+        <v>16120</v>
+      </c>
+      <c r="L217">
         <f t="shared" si="8"/>
-        <v>16120</v>
-      </c>
-      <c r="L217">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10527,11 +10607,11 @@
         <v>217</v>
       </c>
       <c r="K218" s="5">
+        <f t="shared" si="9"/>
+        <v>16130</v>
+      </c>
+      <c r="L218">
         <f t="shared" si="8"/>
-        <v>16130</v>
-      </c>
-      <c r="L218">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10567,11 +10647,11 @@
         <v>218</v>
       </c>
       <c r="K219" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>03600</v>
+      </c>
+      <c r="L219">
         <f t="shared" si="8"/>
-        <v>03600</v>
-      </c>
-      <c r="L219">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10607,11 +10687,11 @@
         <v>219</v>
       </c>
       <c r="K220" s="5">
+        <f t="shared" si="9"/>
+        <v>12000</v>
+      </c>
+      <c r="L220">
         <f t="shared" si="8"/>
-        <v>12000</v>
-      </c>
-      <c r="L220">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10647,11 +10727,11 @@
         <v>220</v>
       </c>
       <c r="K221" s="5">
+        <f t="shared" si="9"/>
+        <v>12005</v>
+      </c>
+      <c r="L221">
         <f t="shared" si="8"/>
-        <v>12005</v>
-      </c>
-      <c r="L221">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10687,11 +10767,11 @@
         <v>221</v>
       </c>
       <c r="K222" s="5">
+        <f t="shared" si="9"/>
+        <v>12010</v>
+      </c>
+      <c r="L222">
         <f t="shared" si="8"/>
-        <v>12010</v>
-      </c>
-      <c r="L222">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10727,11 +10807,11 @@
         <v>222</v>
       </c>
       <c r="K223" s="5">
+        <f t="shared" si="9"/>
+        <v>12020</v>
+      </c>
+      <c r="L223">
         <f t="shared" si="8"/>
-        <v>12020</v>
-      </c>
-      <c r="L223">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10767,11 +10847,11 @@
         <v>223</v>
       </c>
       <c r="K224" s="5">
+        <f t="shared" si="9"/>
+        <v>12030</v>
+      </c>
+      <c r="L224">
         <f t="shared" si="8"/>
-        <v>12030</v>
-      </c>
-      <c r="L224">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10807,11 +10887,11 @@
         <v>224</v>
       </c>
       <c r="K225" s="5">
+        <f t="shared" si="9"/>
+        <v>12040</v>
+      </c>
+      <c r="L225">
         <f t="shared" si="8"/>
-        <v>12040</v>
-      </c>
-      <c r="L225">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10847,11 +10927,11 @@
         <v>225</v>
       </c>
       <c r="K226" s="5">
+        <f t="shared" si="9"/>
+        <v>12090</v>
+      </c>
+      <c r="L226">
         <f t="shared" si="8"/>
-        <v>12090</v>
-      </c>
-      <c r="L226">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10887,11 +10967,11 @@
         <v>226</v>
       </c>
       <c r="K227" s="5">
+        <f t="shared" si="9"/>
+        <v>21100</v>
+      </c>
+      <c r="L227">
         <f t="shared" si="8"/>
-        <v>21100</v>
-      </c>
-      <c r="L227">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10927,11 +11007,11 @@
         <v>227</v>
       </c>
       <c r="K228" s="5">
+        <f t="shared" si="9"/>
+        <v>10100</v>
+      </c>
+      <c r="L228">
         <f t="shared" si="8"/>
-        <v>10100</v>
-      </c>
-      <c r="L228">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -10967,11 +11047,11 @@
         <v>228</v>
       </c>
       <c r="K229" s="5">
+        <f t="shared" si="9"/>
+        <v>10120</v>
+      </c>
+      <c r="L229">
         <f t="shared" si="8"/>
-        <v>10120</v>
-      </c>
-      <c r="L229">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11007,11 +11087,11 @@
         <v>229</v>
       </c>
       <c r="K230" s="5">
+        <f t="shared" si="9"/>
+        <v>10130</v>
+      </c>
+      <c r="L230">
         <f t="shared" si="8"/>
-        <v>10130</v>
-      </c>
-      <c r="L230">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11047,11 +11127,11 @@
         <v>230</v>
       </c>
       <c r="K231" s="5">
+        <f t="shared" si="9"/>
+        <v>10150</v>
+      </c>
+      <c r="L231">
         <f t="shared" si="8"/>
-        <v>10150</v>
-      </c>
-      <c r="L231">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11087,11 +11167,11 @@
         <v>231</v>
       </c>
       <c r="K232" s="5">
+        <f t="shared" si="9"/>
+        <v>10205</v>
+      </c>
+      <c r="L232">
         <f t="shared" si="8"/>
-        <v>10205</v>
-      </c>
-      <c r="L232">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11127,11 +11207,11 @@
         <v>232</v>
       </c>
       <c r="K233" s="5">
+        <f t="shared" si="9"/>
+        <v>10225</v>
+      </c>
+      <c r="L233">
         <f t="shared" si="8"/>
-        <v>10225</v>
-      </c>
-      <c r="L233">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11167,11 +11247,11 @@
         <v>233</v>
       </c>
       <c r="K234" s="5">
+        <f t="shared" si="9"/>
+        <v>10300</v>
+      </c>
+      <c r="L234">
         <f t="shared" si="8"/>
-        <v>10300</v>
-      </c>
-      <c r="L234">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11207,11 +11287,11 @@
         <v>234</v>
       </c>
       <c r="K235" s="5">
+        <f t="shared" si="9"/>
+        <v>10310</v>
+      </c>
+      <c r="L235">
         <f t="shared" si="8"/>
-        <v>10310</v>
-      </c>
-      <c r="L235">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11247,11 +11327,11 @@
         <v>235</v>
       </c>
       <c r="K236" s="5">
+        <f t="shared" si="9"/>
+        <v>10600</v>
+      </c>
+      <c r="L236">
         <f t="shared" si="8"/>
-        <v>10600</v>
-      </c>
-      <c r="L236">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11287,11 +11367,11 @@
         <v>236</v>
       </c>
       <c r="K237" s="5">
+        <f t="shared" si="9"/>
+        <v>10900</v>
+      </c>
+      <c r="L237">
         <f t="shared" si="8"/>
-        <v>10900</v>
-      </c>
-      <c r="L237">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11327,11 +11407,11 @@
         <v>237</v>
       </c>
       <c r="K238" s="5">
+        <f t="shared" si="9"/>
+        <v>10910</v>
+      </c>
+      <c r="L238">
         <f t="shared" si="8"/>
-        <v>10910</v>
-      </c>
-      <c r="L238">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11367,11 +11447,11 @@
         <v>238</v>
       </c>
       <c r="K239" s="5">
+        <f t="shared" si="9"/>
+        <v>10110</v>
+      </c>
+      <c r="L239">
         <f t="shared" si="8"/>
-        <v>10110</v>
-      </c>
-      <c r="L239">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11407,11 +11487,11 @@
         <v>239</v>
       </c>
       <c r="K240" s="5">
+        <f t="shared" si="9"/>
+        <v>10215</v>
+      </c>
+      <c r="L240">
         <f t="shared" si="8"/>
-        <v>10215</v>
-      </c>
-      <c r="L240">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11447,11 +11527,11 @@
         <v>240</v>
       </c>
       <c r="K241" s="5">
+        <f t="shared" si="9"/>
+        <v>10000</v>
+      </c>
+      <c r="L241">
         <f t="shared" si="8"/>
-        <v>10000</v>
-      </c>
-      <c r="L241">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11487,11 +11567,11 @@
         <v>241</v>
       </c>
       <c r="K242" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>04000</v>
+      </c>
+      <c r="L242">
         <f t="shared" si="8"/>
-        <v>04000</v>
-      </c>
-      <c r="L242">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11527,11 +11607,11 @@
         <v>242</v>
       </c>
       <c r="K243" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>04110</v>
+      </c>
+      <c r="L243">
         <f t="shared" si="8"/>
-        <v>04110</v>
-      </c>
-      <c r="L243">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11567,11 +11647,11 @@
         <v>243</v>
       </c>
       <c r="K244" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>04180</v>
+      </c>
+      <c r="L244">
         <f t="shared" si="8"/>
-        <v>04180</v>
-      </c>
-      <c r="L244">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11607,11 +11687,11 @@
         <v>244</v>
       </c>
       <c r="K245" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>04100</v>
+      </c>
+      <c r="L245">
         <f t="shared" si="8"/>
-        <v>04100</v>
-      </c>
-      <c r="L245">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11647,11 +11727,11 @@
         <v>245</v>
       </c>
       <c r="K246" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>04181</v>
+      </c>
+      <c r="L246">
         <f t="shared" si="8"/>
-        <v>04181</v>
-      </c>
-      <c r="L246">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11684,11 +11764,11 @@
         <v>246</v>
       </c>
       <c r="K247" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>04190</v>
+      </c>
+      <c r="L247">
         <f t="shared" si="8"/>
-        <v>04190</v>
-      </c>
-      <c r="L247">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11724,11 +11804,11 @@
         <v>247</v>
       </c>
       <c r="K248" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>05201</v>
+      </c>
+      <c r="L248">
         <f t="shared" si="8"/>
-        <v>05201</v>
-      </c>
-      <c r="L248">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11764,11 +11844,11 @@
         <v>248</v>
       </c>
       <c r="K249" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>05200</v>
+      </c>
+      <c r="L249">
         <f t="shared" si="8"/>
-        <v>05200</v>
-      </c>
-      <c r="L249">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11804,11 +11884,11 @@
         <v>249</v>
       </c>
       <c r="K250" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>05202</v>
+      </c>
+      <c r="L250">
         <f t="shared" si="8"/>
-        <v>05202</v>
-      </c>
-      <c r="L250">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11844,11 +11924,11 @@
         <v>250</v>
       </c>
       <c r="K251" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>05209</v>
+      </c>
+      <c r="L251">
         <f t="shared" si="8"/>
-        <v>05209</v>
-      </c>
-      <c r="L251">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11881,11 +11961,11 @@
         <v>251</v>
       </c>
       <c r="K252" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>06000</v>
+      </c>
+      <c r="L252">
         <f t="shared" si="8"/>
-        <v>06000</v>
-      </c>
-      <c r="L252">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11918,11 +11998,11 @@
         <v>252</v>
       </c>
       <c r="K253" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>06100</v>
+      </c>
+      <c r="L253">
         <f t="shared" si="8"/>
-        <v>06100</v>
-      </c>
-      <c r="L253">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11958,11 +12038,11 @@
         <v>253</v>
       </c>
       <c r="K254" s="5">
+        <f t="shared" si="9"/>
+        <v>13000</v>
+      </c>
+      <c r="L254">
         <f t="shared" si="8"/>
-        <v>13000</v>
-      </c>
-      <c r="L254">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -11998,11 +12078,11 @@
         <v>254</v>
       </c>
       <c r="K255" s="5">
+        <f t="shared" si="9"/>
+        <v>13001</v>
+      </c>
+      <c r="L255">
         <f t="shared" si="8"/>
-        <v>13001</v>
-      </c>
-      <c r="L255">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -12038,11 +12118,11 @@
         <v>255</v>
       </c>
       <c r="K256" s="5">
+        <f t="shared" si="9"/>
+        <v>13013</v>
+      </c>
+      <c r="L256">
         <f t="shared" si="8"/>
-        <v>13013</v>
-      </c>
-      <c r="L256">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -12078,11 +12158,11 @@
         <v>256</v>
       </c>
       <c r="K257" s="5">
+        <f t="shared" si="9"/>
+        <v>13014</v>
+      </c>
+      <c r="L257">
         <f t="shared" si="8"/>
-        <v>13014</v>
-      </c>
-      <c r="L257">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -12118,11 +12198,11 @@
         <v>257</v>
       </c>
       <c r="K258" s="5">
+        <f t="shared" si="9"/>
+        <v>13017</v>
+      </c>
+      <c r="L258">
         <f t="shared" si="8"/>
-        <v>13017</v>
-      </c>
-      <c r="L258">
-        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
@@ -12158,11 +12238,11 @@
         <v>258</v>
       </c>
       <c r="K259" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13019</v>
       </c>
       <c r="L259">
-        <f t="shared" ref="L259:L303" si="9">LEN(K259)</f>
+        <f t="shared" ref="L259:L303" si="10">LEN(K259)</f>
         <v>5</v>
       </c>
     </row>
@@ -12198,11 +12278,11 @@
         <v>259</v>
       </c>
       <c r="K260" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13020</v>
       </c>
       <c r="L260">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -12238,11 +12318,11 @@
         <v>260</v>
       </c>
       <c r="K261" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13021</v>
       </c>
       <c r="L261">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -12278,11 +12358,11 @@
         <v>261</v>
       </c>
       <c r="K262" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13022</v>
       </c>
       <c r="L262">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -12318,11 +12398,11 @@
         <v>262</v>
       </c>
       <c r="K263" s="5">
-        <f t="shared" ref="K263:K303" si="10">IF(LEN(A263)&lt;5,"0"&amp;A263,A263)</f>
+        <f t="shared" ref="K263:K303" si="11">IF(LEN(A263)&lt;5,"0"&amp;A263,A263)</f>
         <v>13030</v>
       </c>
       <c r="L263">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -12358,11 +12438,11 @@
         <v>263</v>
       </c>
       <c r="K264" s="5">
+        <f t="shared" si="11"/>
+        <v>13040</v>
+      </c>
+      <c r="L264">
         <f t="shared" si="10"/>
-        <v>13040</v>
-      </c>
-      <c r="L264">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12398,11 +12478,11 @@
         <v>264</v>
       </c>
       <c r="K265" s="5">
+        <f t="shared" si="11"/>
+        <v>13050</v>
+      </c>
+      <c r="L265">
         <f t="shared" si="10"/>
-        <v>13050</v>
-      </c>
-      <c r="L265">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12438,11 +12518,11 @@
         <v>265</v>
       </c>
       <c r="K266" s="5">
+        <f t="shared" si="11"/>
+        <v>13099</v>
+      </c>
+      <c r="L266">
         <f t="shared" si="10"/>
-        <v>13099</v>
-      </c>
-      <c r="L266">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12478,11 +12558,11 @@
         <v>266</v>
       </c>
       <c r="K267" s="5">
+        <f t="shared" si="11"/>
+        <v>13100</v>
+      </c>
+      <c r="L267">
         <f t="shared" si="10"/>
-        <v>13100</v>
-      </c>
-      <c r="L267">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12518,11 +12598,11 @@
         <v>267</v>
       </c>
       <c r="K268" s="5">
+        <f t="shared" si="11"/>
+        <v>13200</v>
+      </c>
+      <c r="L268">
         <f t="shared" si="10"/>
-        <v>13200</v>
-      </c>
-      <c r="L268">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12558,11 +12638,11 @@
         <v>268</v>
       </c>
       <c r="K269" s="5">
+        <f t="shared" si="11"/>
+        <v>12200</v>
+      </c>
+      <c r="L269">
         <f t="shared" si="10"/>
-        <v>12200</v>
-      </c>
-      <c r="L269">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12598,11 +12678,11 @@
         <v>269</v>
       </c>
       <c r="K270" s="5">
+        <f t="shared" si="11"/>
+        <v>12100</v>
+      </c>
+      <c r="L270">
         <f t="shared" si="10"/>
-        <v>12100</v>
-      </c>
-      <c r="L270">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12638,11 +12718,11 @@
         <v>270</v>
       </c>
       <c r="K271" s="5">
+        <f t="shared" si="11"/>
+        <v>14010</v>
+      </c>
+      <c r="L271">
         <f t="shared" si="10"/>
-        <v>14010</v>
-      </c>
-      <c r="L271">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12678,11 +12758,11 @@
         <v>271</v>
       </c>
       <c r="K272" s="5">
+        <f t="shared" si="11"/>
+        <v>14600</v>
+      </c>
+      <c r="L272">
         <f t="shared" si="10"/>
-        <v>14600</v>
-      </c>
-      <c r="L272">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12718,11 +12798,11 @@
         <v>272</v>
       </c>
       <c r="K273" s="5">
+        <f t="shared" si="11"/>
+        <v>14610</v>
+      </c>
+      <c r="L273">
         <f t="shared" si="10"/>
-        <v>14610</v>
-      </c>
-      <c r="L273">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12758,11 +12838,11 @@
         <v>273</v>
       </c>
       <c r="K274" s="5">
+        <f t="shared" si="11"/>
+        <v>14620</v>
+      </c>
+      <c r="L274">
         <f t="shared" si="10"/>
-        <v>14620</v>
-      </c>
-      <c r="L274">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12798,11 +12878,11 @@
         <v>274</v>
       </c>
       <c r="K275" s="5">
+        <f t="shared" si="11"/>
+        <v>14621</v>
+      </c>
+      <c r="L275">
         <f t="shared" si="10"/>
-        <v>14621</v>
-      </c>
-      <c r="L275">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12838,11 +12918,11 @@
         <v>275</v>
       </c>
       <c r="K276" s="5">
+        <f t="shared" si="11"/>
+        <v>14622</v>
+      </c>
+      <c r="L276">
         <f t="shared" si="10"/>
-        <v>14622</v>
-      </c>
-      <c r="L276">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12878,11 +12958,11 @@
         <v>276</v>
       </c>
       <c r="K277" s="5">
+        <f t="shared" si="11"/>
+        <v>14630</v>
+      </c>
+      <c r="L277">
         <f t="shared" si="10"/>
-        <v>14630</v>
-      </c>
-      <c r="L277">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12918,11 +12998,11 @@
         <v>277</v>
       </c>
       <c r="K278" s="5">
+        <f t="shared" si="11"/>
+        <v>14660</v>
+      </c>
+      <c r="L278">
         <f t="shared" si="10"/>
-        <v>14660</v>
-      </c>
-      <c r="L278">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12958,11 +13038,11 @@
         <v>278</v>
       </c>
       <c r="K279" s="5">
+        <f t="shared" si="11"/>
+        <v>14700</v>
+      </c>
+      <c r="L279">
         <f t="shared" si="10"/>
-        <v>14700</v>
-      </c>
-      <c r="L279">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -12998,11 +13078,11 @@
         <v>279</v>
       </c>
       <c r="K280" s="5">
+        <f t="shared" si="11"/>
+        <v>14710</v>
+      </c>
+      <c r="L280">
         <f t="shared" si="10"/>
-        <v>14710</v>
-      </c>
-      <c r="L280">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13038,11 +13118,11 @@
         <v>280</v>
       </c>
       <c r="K281" s="5">
+        <f t="shared" si="11"/>
+        <v>14720</v>
+      </c>
+      <c r="L281">
         <f t="shared" si="10"/>
-        <v>14720</v>
-      </c>
-      <c r="L281">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13078,11 +13158,11 @@
         <v>281</v>
       </c>
       <c r="K282" s="5">
+        <f t="shared" si="11"/>
+        <v>14730</v>
+      </c>
+      <c r="L282">
         <f t="shared" si="10"/>
-        <v>14730</v>
-      </c>
-      <c r="L282">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13118,11 +13198,11 @@
         <v>282</v>
       </c>
       <c r="K283" s="5">
+        <f t="shared" si="11"/>
+        <v>14740</v>
+      </c>
+      <c r="L283">
         <f t="shared" si="10"/>
-        <v>14740</v>
-      </c>
-      <c r="L283">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13158,11 +13238,11 @@
         <v>283</v>
       </c>
       <c r="K284" s="5">
+        <f t="shared" si="11"/>
+        <v>14755</v>
+      </c>
+      <c r="L284">
         <f t="shared" si="10"/>
-        <v>14755</v>
-      </c>
-      <c r="L284">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13198,11 +13278,11 @@
         <v>284</v>
       </c>
       <c r="K285" s="5">
+        <f t="shared" si="11"/>
+        <v>14765</v>
+      </c>
+      <c r="L285">
         <f t="shared" si="10"/>
-        <v>14765</v>
-      </c>
-      <c r="L285">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13238,11 +13318,11 @@
         <v>285</v>
       </c>
       <c r="K286" s="5">
+        <f t="shared" si="11"/>
+        <v>17000</v>
+      </c>
+      <c r="L286">
         <f t="shared" si="10"/>
-        <v>17000</v>
-      </c>
-      <c r="L286">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13278,11 +13358,11 @@
         <v>286</v>
       </c>
       <c r="K287" s="5">
+        <f t="shared" si="11"/>
+        <v>17010</v>
+      </c>
+      <c r="L287">
         <f t="shared" si="10"/>
-        <v>17010</v>
-      </c>
-      <c r="L287">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13318,11 +13398,11 @@
         <v>287</v>
       </c>
       <c r="K288" s="5">
+        <f t="shared" si="11"/>
+        <v>17020</v>
+      </c>
+      <c r="L288">
         <f t="shared" si="10"/>
-        <v>17020</v>
-      </c>
-      <c r="L288">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13358,11 +13438,11 @@
         <v>288</v>
       </c>
       <c r="K289" s="5">
+        <f t="shared" si="11"/>
+        <v>17030</v>
+      </c>
+      <c r="L289">
         <f t="shared" si="10"/>
-        <v>17030</v>
-      </c>
-      <c r="L289">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13398,11 +13478,11 @@
         <v>289</v>
       </c>
       <c r="K290" s="5">
+        <f t="shared" si="11"/>
+        <v>17050</v>
+      </c>
+      <c r="L290">
         <f t="shared" si="10"/>
-        <v>17050</v>
-      </c>
-      <c r="L290">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13438,11 +13518,11 @@
         <v>290</v>
       </c>
       <c r="K291" s="5">
+        <f t="shared" si="11"/>
+        <v>17100</v>
+      </c>
+      <c r="L291">
         <f t="shared" si="10"/>
-        <v>17100</v>
-      </c>
-      <c r="L291">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13478,11 +13558,11 @@
         <v>291</v>
       </c>
       <c r="K292" s="5">
+        <f t="shared" si="11"/>
+        <v>17110</v>
+      </c>
+      <c r="L292">
         <f t="shared" si="10"/>
-        <v>17110</v>
-      </c>
-      <c r="L292">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13518,11 +13598,11 @@
         <v>292</v>
       </c>
       <c r="K293" s="5">
+        <f t="shared" si="11"/>
+        <v>17120</v>
+      </c>
+      <c r="L293">
         <f t="shared" si="10"/>
-        <v>17120</v>
-      </c>
-      <c r="L293">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13558,11 +13638,11 @@
         <v>293</v>
       </c>
       <c r="K294" s="5">
+        <f t="shared" si="11"/>
+        <v>18010</v>
+      </c>
+      <c r="L294">
         <f t="shared" si="10"/>
-        <v>18010</v>
-      </c>
-      <c r="L294">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13598,11 +13678,11 @@
         <v>294</v>
       </c>
       <c r="K295" s="5">
+        <f t="shared" si="11"/>
+        <v>18100</v>
+      </c>
+      <c r="L295">
         <f t="shared" si="10"/>
-        <v>18100</v>
-      </c>
-      <c r="L295">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13638,11 +13718,11 @@
         <v>295</v>
       </c>
       <c r="K296" s="5">
+        <f t="shared" si="11"/>
+        <v>18110</v>
+      </c>
+      <c r="L296">
         <f t="shared" si="10"/>
-        <v>18110</v>
-      </c>
-      <c r="L296">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13678,11 +13758,11 @@
         <v>296</v>
       </c>
       <c r="K297" s="5">
+        <f t="shared" si="11"/>
+        <v>20100</v>
+      </c>
+      <c r="L297">
         <f t="shared" si="10"/>
-        <v>20100</v>
-      </c>
-      <c r="L297">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13718,11 +13798,11 @@
         <v>297</v>
       </c>
       <c r="K298" s="5">
+        <f t="shared" si="11"/>
+        <v>20200</v>
+      </c>
+      <c r="L298">
         <f t="shared" si="10"/>
-        <v>20200</v>
-      </c>
-      <c r="L298">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13758,11 +13838,11 @@
         <v>298</v>
       </c>
       <c r="K299" s="5">
+        <f t="shared" si="11"/>
+        <v>20300</v>
+      </c>
+      <c r="L299">
         <f t="shared" si="10"/>
-        <v>20300</v>
-      </c>
-      <c r="L299">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13798,11 +13878,11 @@
         <v>299</v>
       </c>
       <c r="K300" s="5">
+        <f t="shared" si="11"/>
+        <v>20400</v>
+      </c>
+      <c r="L300">
         <f t="shared" si="10"/>
-        <v>20400</v>
-      </c>
-      <c r="L300">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13838,11 +13918,11 @@
         <v>300</v>
       </c>
       <c r="K301" s="5">
+        <f t="shared" si="11"/>
+        <v>21000</v>
+      </c>
+      <c r="L301">
         <f t="shared" si="10"/>
-        <v>21000</v>
-      </c>
-      <c r="L301">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13878,11 +13958,11 @@
         <v>301</v>
       </c>
       <c r="K302" s="5">
+        <f t="shared" si="11"/>
+        <v>21200</v>
+      </c>
+      <c r="L302">
         <f t="shared" si="10"/>
-        <v>21200</v>
-      </c>
-      <c r="L302">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -13918,11 +13998,11 @@
         <v>302</v>
       </c>
       <c r="K303" s="5">
+        <f t="shared" si="11"/>
+        <v>21300</v>
+      </c>
+      <c r="L303">
         <f t="shared" si="10"/>
-        <v>21300</v>
-      </c>
-      <c r="L303">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -14303,6 +14383,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<json>
+  <seTables>
+{
+  "Settings": [],
+  "tables": []
+}
+</seTables>
+</json>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054C67748DE492541BD81094B81368739" ma:contentTypeVersion="16" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4463fa060f78a3f9a5c5eff72e026175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ce2bc919-6586-4803-b73a-5706cf1a1a01" xmlns:ns3="10fc2a72-d6c9-426a-a62e-2f32029c34a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d37a0e132dfaa5c89d8f6c8e41d6f78" ns2:_="" ns3:_="">
     <xsd:import namespace="ce2bc919-6586-4803-b73a-5706cf1a1a01"/>
@@ -14549,40 +14649,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<json>
-  <seTables>
-{
-  "Settings": [],
-  "tables": []
-}
-</seTables>
-</json>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce2bc919-6586-4803-b73a-5706cf1a1a01">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <R_x002e_T_x002e_T_x002e_ xmlns="ce2bc919-6586-4803-b73a-5706cf1a1a01">Nee</R_x002e_T_x002e_T_x002e_>
-    <TaxCatchAll xmlns="10fc2a72-d6c9-426a-a62e-2f32029c34a1" xsi:nil="true"/>
-    <Status xmlns="ce2bc919-6586-4803-b73a-5706cf1a1a01">ONTW</Status>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <json>
   <seSettings>
 {
@@ -14597,7 +14664,34 @@
 </json>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ce2bc919-6586-4803-b73a-5706cf1a1a01">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <R_x002e_T_x002e_T_x002e_ xmlns="ce2bc919-6586-4803-b73a-5706cf1a1a01">Nee</R_x002e_T_x002e_T_x002e_>
+    <TaxCatchAll xmlns="10fc2a72-d6c9-426a-a62e-2f32029c34a1" xsi:nil="true"/>
+    <Status xmlns="ce2bc919-6586-4803-b73a-5706cf1a1a01">ONTW</Status>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA18ACFC-59D7-4607-A1B1-D54C7169526E}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E4A638D-DAA1-4526-918D-79D6C8F02C3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4236CD60-8641-4A25-9136-7ECB41A01D83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14616,21 +14710,13 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E4A638D-DAA1-4526-918D-79D6C8F02C3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA18ACFC-59D7-4607-A1B1-D54C7169526E}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90555017-C3BF-4A4E-9652-1F5FBBD8A4AA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B153D69-EE67-422F-B3AE-3A7AD49B1B39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14639,10 +14725,4 @@
     <ds:schemaRef ds:uri="10fc2a72-d6c9-426a-a62e-2f32029c34a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90555017-C3BF-4A4E-9652-1F5FBBD8A4AA}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>